<commit_message>
Finished Initial Version + ErrorLog Monitoring w/ PowerShell
</commit_message>
<xml_diff>
--- a/Bulk Loads/0923/_PRELIMINARY UTILITY EXPORT - FS_formatted.xlsx
+++ b/Bulk Loads/0923/_PRELIMINARY UTILITY EXPORT - FS_formatted.xlsx
@@ -481,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:S100"/>
+  <dimension ref="A3:S101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
@@ -514,7 +514,7 @@
     <row r="4" ht="27" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>August 05, 2024</t>
+          <t>August 07, 2024</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="5" t="n">
-        <v>17.5</v>
+        <v>16</v>
       </c>
       <c r="G30" s="6">
         <f>IF(E30&gt;1,(1.732*D30*F30)/1000,(D30*F30)/1000)</f>
@@ -1241,163 +1241,177 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" t="n">
         <v>1</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>FRONT SERVING COUNTER</t>
-        </is>
-      </c>
-      <c r="F31" s="5" t="n"/>
-      <c r="G31" s="6" t="n"/>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>CUSTOM FABRICATION</t>
+          <t>REFRIGERATED GRAB &amp; GO CASE</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>120</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G31" s="6">
+        <f>IF(E31&gt;1,(1.732*D31*F31)/1000,(D31*F31)/1000)</f>
+        <v/>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>1 1/2"</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>POS SYSTEM</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>120</v>
-      </c>
-      <c r="E32" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="G32" s="6">
-        <f>IF(E32&gt;1,(1.732*D32*F32)/1000,(D32*F32)/1000)</f>
-        <v/>
-      </c>
+          <t>FRONT SERVING COUNTER</t>
+        </is>
+      </c>
+      <c r="F32" s="5" t="n"/>
+      <c r="G32" s="6" t="n"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>BY OS&amp;E</t>
+          <t>CUSTOM FABRICATION</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>25</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>24</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
-        </is>
-      </c>
-      <c r="F33" s="5" t="n"/>
-      <c r="G33" s="6" t="n"/>
+          <t>POS SYSTEM</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>120</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="G33" s="6">
+        <f>IF(E33&gt;1,(1.732*D33*F33)/1000,(D33*F33)/1000)</f>
+        <v/>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>BY OS&amp;E</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>26</v>
-      </c>
-      <c r="B34" t="n">
-        <v>2</v>
+        <v>25</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>POS PRINTER</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>120</v>
-      </c>
-      <c r="E34" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="G34" s="6">
-        <f>IF(E34&gt;1,(1.732*D34*F34)/1000,(D34*F34)/1000)</f>
-        <v/>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>BY OS&amp;E</t>
-        </is>
-      </c>
+          <t>SPARE NUMBER</t>
+        </is>
+      </c>
+      <c r="F34" s="5" t="n"/>
+      <c r="G34" s="6" t="n"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>TEA WIRE RACK</t>
-        </is>
-      </c>
-      <c r="F35" s="5" t="n"/>
-      <c r="G35" s="6" t="n"/>
+          <t>POS PRINTER</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>120</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G35" s="6">
+        <f>IF(E35&gt;1,(1.732*D35*F35)/1000,(D35*F35)/1000)</f>
+        <v/>
+      </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>BY VENDOR</t>
+          <t>BY OS&amp;E</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" t="n">
         <v>1</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TRASH RECEPTACLE</t>
+          <t>TEA WIRE RACK</t>
         </is>
       </c>
       <c r="F36" s="5" t="n"/>
       <c r="G36" s="6" t="n"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>SLIM JIM</t>
+          <t>BY VENDOR</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>29</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>28</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
+          <t>TRASH RECEPTACLE</t>
         </is>
       </c>
       <c r="F37" s="5" t="n"/>
       <c r="G37" s="6" t="n"/>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>SLIM JIM</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1414,213 +1428,213 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>31</v>
-      </c>
-      <c r="B39" t="n">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>KNOCK BOX</t>
+          <t>SPARE NUMBER</t>
         </is>
       </c>
       <c r="F39" s="5" t="n"/>
       <c r="G39" s="6" t="n"/>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>CUSTOM FABRICATION PART OF ITEM #23</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" t="n">
         <v>1</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SYRUP WIRE RACK</t>
+          <t>KNOCK BOX</t>
         </is>
       </c>
       <c r="F40" s="5" t="n"/>
       <c r="G40" s="6" t="n"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>BY VENDOR</t>
+          <t>CUSTOM FABRICATION PART OF ITEM #23</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B41" t="n">
         <v>1</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>UNDERCOUNTER FREEZER</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>120</v>
-      </c>
-      <c r="E41" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G41" s="6">
-        <f>IF(E41&gt;1,(1.732*D41*F41)/1000,(D41*F41)/1000)</f>
-        <v/>
-      </c>
+          <t>SYRUP WIRE RACK</t>
+        </is>
+      </c>
+      <c r="F41" s="5" t="n"/>
+      <c r="G41" s="6" t="n"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>MOBILE</t>
+          <t>BY VENDOR</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B42" t="n">
         <v>1</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ACRYLIC SURROUND</t>
-        </is>
-      </c>
-      <c r="F42" s="5" t="n"/>
-      <c r="G42" s="6" t="n"/>
+          <t>UNDERCOUNTER FREEZER</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>120</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G42" s="6">
+        <f>IF(E42&gt;1,(1.732*D42*F42)/1000,(D42*F42)/1000)</f>
+        <v/>
+      </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>MILLWORK / BY GENERAL CONTRACTOR</t>
+          <t>MOBILE</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>35</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>34</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
+          <t>ACRYLIC SURROUND</t>
         </is>
       </c>
       <c r="F43" s="5" t="n"/>
       <c r="G43" s="6" t="n"/>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>MILLWORK / BY GENERAL CONTRACTOR</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>36</v>
-      </c>
-      <c r="B44" t="n">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>SAUCE WIRE RACK</t>
+          <t>SPARE NUMBER</t>
         </is>
       </c>
       <c r="F44" s="5" t="n"/>
       <c r="G44" s="6" t="n"/>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>BY VENDOR</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" t="n">
         <v>1</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ESPRESSO MACHINE</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>208</v>
-      </c>
-      <c r="E45" t="n">
-        <v>3</v>
-      </c>
-      <c r="F45" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="G45" s="6">
-        <f>IF(E45&gt;1,(1.732*D45*F45)/1000,(D45*F45)/1000)</f>
-        <v/>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>3/8"</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>1 1/2"</t>
+          <t>SAUCE WIRE RACK</t>
+        </is>
+      </c>
+      <c r="F45" s="5" t="n"/>
+      <c r="G45" s="6" t="n"/>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>BY VENDOR</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46" t="n">
         <v>1</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>DRIP TROUGH</t>
-        </is>
-      </c>
-      <c r="F46" s="5" t="n"/>
-      <c r="G46" s="6" t="n"/>
+          <t>ESPRESSO MACHINE</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>208</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3</v>
+      </c>
+      <c r="F46" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="G46" s="6">
+        <f>IF(E46&gt;1,(1.732*D46*F46)/1000,(D46*F46)/1000)</f>
+        <v/>
+      </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>3/8"</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>1 1/2"</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>39</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>38</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
+          <t>DRIP TROUGH</t>
         </is>
       </c>
       <c r="F47" s="5" t="n"/>
       <c r="G47" s="6" t="n"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>1/2"</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>1/2"</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1637,39 +1651,31 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>41</v>
-      </c>
-      <c r="B49" t="n">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>WATER STATION</t>
+          <t>SPARE NUMBER</t>
         </is>
       </c>
       <c r="F49" s="5" t="n"/>
       <c r="G49" s="6" t="n"/>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>1/2"</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>1 1/4"</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50" t="n">
         <v>1</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>DIPPERWELL</t>
+          <t>WATER STATION</t>
         </is>
       </c>
       <c r="F50" s="5" t="n"/>
@@ -1681,61 +1687,69 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>1-1/2"</t>
+          <t>1 1/4"</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51" t="n">
         <v>1</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>UNDERCOUNTER REFRIGERATOR</t>
-        </is>
-      </c>
-      <c r="D51" t="n">
-        <v>120</v>
-      </c>
-      <c r="E51" t="n">
-        <v>1</v>
-      </c>
-      <c r="F51" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G51" s="6">
-        <f>IF(E51&gt;1,(1.732*D51*F51)/1000,(D51*F51)/1000)</f>
-        <v/>
-      </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>MOBILE</t>
+          <t>DIPPERWELL</t>
+        </is>
+      </c>
+      <c r="F51" s="5" t="n"/>
+      <c r="G51" s="6" t="n"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>1/2"</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>1-1/2"</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>44</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>43</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
-        </is>
-      </c>
-      <c r="F52" s="5" t="n"/>
-      <c r="G52" s="6" t="n"/>
+          <t>UNDERCOUNTER REFRIGERATOR</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>120</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G52" s="6">
+        <f>IF(E52&gt;1,(1.732*D52*F52)/1000,(D52*F52)/1000)</f>
+        <v/>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>MOBILE</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1752,45 +1766,31 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>46</v>
-      </c>
-      <c r="B54" t="n">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>FREEZER MERCHANDISER</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>120</v>
-      </c>
-      <c r="E54" t="n">
-        <v>1</v>
-      </c>
-      <c r="F54" s="5" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="G54" s="6">
-        <f>IF(E54&gt;1,(1.732*D54*F54)/1000,(D54*F54)/1000)</f>
-        <v/>
-      </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>MOBILE</t>
-        </is>
-      </c>
+          <t>SPARE NUMBER</t>
+        </is>
+      </c>
+      <c r="F54" s="5" t="n"/>
+      <c r="G54" s="6" t="n"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>REFRIGERATED MERCHANDISER</t>
+          <t>FREEZER MERCHANDISER</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1800,7 +1800,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="5" t="n">
-        <v>3.1</v>
+        <v>4.6</v>
       </c>
       <c r="G55" s="6">
         <f>IF(E55&gt;1,(1.732*D55*F55)/1000,(D55*F55)/1000)</f>
@@ -1814,14 +1814,14 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>OPEN DISPLAY MERCHANDISER</t>
+          <t>REFRIGERATED MERCHANDISER</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1831,33 +1831,47 @@
         <v>1</v>
       </c>
       <c r="F56" s="5" t="n">
-        <v>16.9</v>
+        <v>3.1</v>
       </c>
       <c r="G56" s="6">
         <f>IF(E56&gt;1,(1.732*D56*F56)/1000,(D56*F56)/1000)</f>
         <v/>
       </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>MOBILE</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>49</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>48</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
-        </is>
-      </c>
-      <c r="F57" s="5" t="n"/>
-      <c r="G57" s="6" t="n"/>
+          <t>OPEN DISPLAY MERCHANDISER</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>120</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" s="5" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="G57" s="6">
+        <f>IF(E57&gt;1,(1.732*D57*F57)/1000,(D57*F57)/1000)</f>
+        <v/>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -1874,69 +1888,71 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>51</v>
-      </c>
-      <c r="B59" t="n">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>TRASH CHUTE</t>
+          <t>SPARE NUMBER</t>
         </is>
       </c>
       <c r="F59" s="5" t="n"/>
       <c r="G59" s="6" t="n"/>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>CUSTOM FABRICATION PART OF ITEM #63</t>
-        </is>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B60" t="n">
         <v>1</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>TRASH RECEPTACLE</t>
+          <t>TRASH CHUTE</t>
         </is>
       </c>
       <c r="F60" s="5" t="n"/>
       <c r="G60" s="6" t="n"/>
       <c r="S60" t="inlineStr">
         <is>
-          <t>SLIM JIM</t>
+          <t>CUSTOM FABRICATION PART OF ITEM #63</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B61" t="n">
         <v>1</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>PAPER NAPKIN DISPENSER</t>
+          <t>TRASH RECEPTACLE</t>
         </is>
       </c>
       <c r="F61" s="5" t="n"/>
       <c r="G61" s="6" t="n"/>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>SLIM JIM</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B62" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>AIRPOT</t>
+          <t>PAPER NAPKIN DISPENSER</t>
         </is>
       </c>
       <c r="F62" s="5" t="n"/>
@@ -1944,16 +1960,14 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>55</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>54</v>
+      </c>
+      <c r="B63" t="n">
+        <v>3</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
+          <t>AIRPOT</t>
         </is>
       </c>
       <c r="F63" s="5" t="n"/>
@@ -1961,14 +1975,16 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>56</v>
-      </c>
-      <c r="B64" t="n">
-        <v>2</v>
+        <v>55</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CONDIMENT CADDY</t>
+          <t>SPARE NUMBER</t>
         </is>
       </c>
       <c r="F64" s="5" t="n"/>
@@ -1976,64 +1992,62 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>TRASH RECEPTACLE</t>
+          <t>CONDIMENT CADDY</t>
         </is>
       </c>
       <c r="F65" s="5" t="n"/>
       <c r="G65" s="6" t="n"/>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>SLIM JIM</t>
-        </is>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B66" t="n">
         <v>1</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>TRASH CHUTE</t>
+          <t>TRASH RECEPTACLE</t>
         </is>
       </c>
       <c r="F66" s="5" t="n"/>
       <c r="G66" s="6" t="n"/>
       <c r="S66" t="inlineStr">
         <is>
-          <t>CUSTOM FABRICATION PART OF ITEM #63</t>
+          <t>SLIM JIM</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>59</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>58</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
+          <t>TRASH CHUTE</t>
         </is>
       </c>
       <c r="F67" s="5" t="n"/>
       <c r="G67" s="6" t="n"/>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>CUSTOM FABRICATION PART OF ITEM #63</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2050,45 +2064,31 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>61</v>
-      </c>
-      <c r="B69" t="n">
-        <v>2</v>
+        <v>60</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SELF-PAY POS SYSTEM</t>
-        </is>
-      </c>
-      <c r="D69" t="n">
-        <v>120</v>
-      </c>
-      <c r="E69" t="n">
-        <v>1</v>
-      </c>
-      <c r="F69" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="G69" s="6">
-        <f>IF(E69&gt;1,(1.732*D69*F69)/1000,(D69*F69)/1000)</f>
-        <v/>
-      </c>
-      <c r="S69" t="inlineStr">
-        <is>
-          <t>BY OS&amp;E</t>
-        </is>
-      </c>
+          <t>SPARE NUMBER</t>
+        </is>
+      </c>
+      <c r="F69" s="5" t="n"/>
+      <c r="G69" s="6" t="n"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B70" t="n">
         <v>2</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>POS PRINTER</t>
+          <t>SELF-PAY POS SYSTEM</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2098,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="5" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G70" s="6">
         <f>IF(E70&gt;1,(1.732*D70*F70)/1000,(D70*F70)/1000)</f>
@@ -2112,14 +2112,14 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SELF CHECK-OUT COUNTER</t>
+          <t>POS PRINTER</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2129,7 +2129,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="5" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G71" s="6">
         <f>IF(E71&gt;1,(1.732*D71*F71)/1000,(D71*F71)/1000)</f>
@@ -2137,24 +2137,35 @@
       </c>
       <c r="S71" t="inlineStr">
         <is>
-          <t>CUSTOM FABRICATION</t>
+          <t>BY OS&amp;E</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B72" t="n">
         <v>1</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SNACK SHELVING</t>
-        </is>
-      </c>
-      <c r="F72" s="5" t="n"/>
-      <c r="G72" s="6" t="n"/>
+          <t>SELF CHECK-OUT COUNTER</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>120</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="G72" s="6">
+        <f>IF(E72&gt;1,(1.732*D72*F72)/1000,(D72*F72)/1000)</f>
+        <v/>
+      </c>
       <c r="S72" t="inlineStr">
         <is>
           <t>CUSTOM FABRICATION</t>
@@ -2163,31 +2174,36 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>65</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>64</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
+          <t>SNACK SHELVING</t>
         </is>
       </c>
       <c r="F73" s="5" t="n"/>
       <c r="G73" s="6" t="n"/>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>CUSTOM FABRICATION</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>66</v>
-      </c>
-      <c r="B74" t="n">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ROBOBURGER MACHINE</t>
+          <t>SPARE NUMBER</t>
         </is>
       </c>
       <c r="F74" s="5" t="n"/>
@@ -2195,47 +2211,39 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B75" t="n">
         <v>1</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>SOFT SERVE ICE CREAM VENDING MACHINE</t>
-        </is>
-      </c>
-      <c r="D75" t="n">
-        <v>208</v>
-      </c>
-      <c r="E75" t="n">
-        <v>1</v>
-      </c>
-      <c r="F75" s="5" t="n">
-        <v>25</v>
-      </c>
+          <t>ROBOBURGER MACHINE</t>
+        </is>
+      </c>
+      <c r="F75" s="5" t="n"/>
       <c r="G75" s="6" t="n"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B76" t="n">
         <v>1</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>HOT FOOD VENDING MACHINE</t>
-        </is>
-      </c>
-      <c r="D76" s="7" t="n">
-        <v>260</v>
+          <t>SOFT SERVE ICE CREAM VENDING MACHINE</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>208</v>
       </c>
       <c r="E76" t="n">
         <v>1</v>
       </c>
       <c r="F76" s="5" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G76" s="6">
         <f>IF(E76&gt;1,(1.732*D76*F76)/1000,(D76*F76)/1000)</f>
@@ -2244,67 +2252,76 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>69</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>68</v>
+      </c>
+      <c r="B77" t="n">
+        <v>1</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
-        </is>
-      </c>
-      <c r="F77" s="5" t="n"/>
-      <c r="G77" s="6" t="n"/>
+          <t>HOT FOOD VENDING MACHINE</t>
+        </is>
+      </c>
+      <c r="D77" s="7" t="n">
+        <v>260</v>
+      </c>
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="G77" s="6">
+        <f>IF(E77&gt;1,(1.732*D77*F77)/1000,(D77*F77)/1000)</f>
+        <v/>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>71</v>
-      </c>
-      <c r="B78" t="n">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>PIZZA VENDING MACHINE</t>
-        </is>
-      </c>
-      <c r="D78" s="7" t="n">
-        <v>230</v>
-      </c>
-      <c r="E78" t="n">
-        <v>3</v>
-      </c>
-      <c r="F78" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="G78" s="6">
-        <f>IF(E78&gt;1,(1.732*D78*F78)/1000,(D78*F78)/1000)</f>
-        <v/>
-      </c>
+          <t>SPARE NUMBER</t>
+        </is>
+      </c>
+      <c r="F78" s="5" t="n"/>
+      <c r="G78" s="6" t="n"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>72</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>71</v>
+      </c>
+      <c r="B79" t="n">
+        <v>1</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
-        </is>
-      </c>
-      <c r="F79" s="5" t="n"/>
-      <c r="G79" s="6" t="n"/>
+          <t>PIZZA VENDING MACHINE</t>
+        </is>
+      </c>
+      <c r="D79" s="7" t="n">
+        <v>230</v>
+      </c>
+      <c r="E79" t="n">
+        <v>3</v>
+      </c>
+      <c r="F79" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="G79" s="6">
+        <f>IF(E79&gt;1,(1.732*D79*F79)/1000,(D79*F79)/1000)</f>
+        <v/>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -2321,7 +2338,7 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -2337,10 +2354,8 @@
       <c r="G81" s="6" t="n"/>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>75-80</t>
-        </is>
+      <c r="A82" t="n">
+        <v>74</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -2356,82 +2371,81 @@
       <c r="G82" s="6" t="n"/>
     </row>
     <row r="83">
-      <c r="A83" s="3" t="inlineStr">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>75-80</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>SPARE NUMBER</t>
+        </is>
+      </c>
+      <c r="F83" s="5" t="n"/>
+      <c r="G83" s="6" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="inlineStr">
         <is>
           <t>BACK OF HOUSE AREA</t>
         </is>
       </c>
-      <c r="B83" s="4" t="n"/>
-      <c r="C83" s="4" t="n"/>
-      <c r="D83" s="4" t="n"/>
-      <c r="E83" s="4" t="n"/>
-      <c r="F83" s="4" t="n"/>
-      <c r="G83" s="4" t="n"/>
-      <c r="H83" s="4" t="n"/>
-      <c r="I83" s="4" t="n"/>
-      <c r="J83" s="4" t="n"/>
-      <c r="K83" s="4" t="n"/>
-      <c r="L83" s="4" t="n"/>
-      <c r="M83" s="4" t="n"/>
-      <c r="N83" s="4" t="n"/>
-      <c r="O83" s="4" t="n"/>
-      <c r="P83" s="4" t="n"/>
-      <c r="Q83" s="4" t="n"/>
-      <c r="R83" s="4" t="n"/>
-      <c r="S83" s="4" t="n"/>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>81</v>
-      </c>
-      <c r="B84" t="n">
-        <v>1</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>THREE COMPARTMENT SINK</t>
-        </is>
-      </c>
-      <c r="F84" s="5" t="n"/>
-      <c r="G84" s="6" t="n"/>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>(2)3/4"</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>(2)3/4"</t>
-        </is>
-      </c>
-      <c r="J84" t="n">
-        <v>90</v>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>(3)2"</t>
-        </is>
-      </c>
-      <c r="S84" t="inlineStr">
-        <is>
-          <t>CUSTOM FABRICATION</t>
-        </is>
-      </c>
+      <c r="B84" s="4" t="n"/>
+      <c r="C84" s="4" t="n"/>
+      <c r="D84" s="4" t="n"/>
+      <c r="E84" s="4" t="n"/>
+      <c r="F84" s="4" t="n"/>
+      <c r="G84" s="4" t="n"/>
+      <c r="H84" s="4" t="n"/>
+      <c r="I84" s="4" t="n"/>
+      <c r="J84" s="4" t="n"/>
+      <c r="K84" s="4" t="n"/>
+      <c r="L84" s="4" t="n"/>
+      <c r="M84" s="4" t="n"/>
+      <c r="N84" s="4" t="n"/>
+      <c r="O84" s="4" t="n"/>
+      <c r="P84" s="4" t="n"/>
+      <c r="Q84" s="4" t="n"/>
+      <c r="R84" s="4" t="n"/>
+      <c r="S84" s="4" t="n"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B85" t="n">
         <v>1</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>POT SHELF</t>
+          <t>THREE COMPARTMENT SINK</t>
         </is>
       </c>
       <c r="F85" s="5" t="n"/>
       <c r="G85" s="6" t="n"/>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>(2)3/4"</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>(2)3/4"</t>
+        </is>
+      </c>
+      <c r="J85" t="n">
+        <v>90</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>(3)2"</t>
+        </is>
+      </c>
       <c r="S85" t="inlineStr">
         <is>
           <t>CUSTOM FABRICATION</t>
@@ -2440,45 +2454,34 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B86" t="n">
         <v>1</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>REACH-IN FREEZER</t>
-        </is>
-      </c>
-      <c r="D86" t="n">
-        <v>120</v>
-      </c>
-      <c r="E86" t="n">
-        <v>1</v>
-      </c>
-      <c r="F86" s="5" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="G86" s="6">
-        <f>IF(E86&gt;1,(1.732*D86*F86)/1000,(D86*F86)/1000)</f>
-        <v/>
-      </c>
+          <t>POT SHELF</t>
+        </is>
+      </c>
+      <c r="F86" s="5" t="n"/>
+      <c r="G86" s="6" t="n"/>
       <c r="S86" t="inlineStr">
         <is>
-          <t>MOBILE</t>
+          <t>CUSTOM FABRICATION</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>REACH-IN REFRIGERATOR</t>
+          <t>REACH-IN FREEZER</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2488,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="5" t="n">
-        <v>10.8</v>
+        <v>3.7</v>
       </c>
       <c r="G87" s="6">
         <f>IF(E87&gt;1,(1.732*D87*F87)/1000,(D87*F87)/1000)</f>
@@ -2502,31 +2505,47 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>85</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>84</v>
+      </c>
+      <c r="B88" t="n">
+        <v>2</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
-        </is>
-      </c>
-      <c r="F88" s="5" t="n"/>
-      <c r="G88" s="6" t="n"/>
+          <t>REACH-IN REFRIGERATOR</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>120</v>
+      </c>
+      <c r="E88" t="n">
+        <v>1</v>
+      </c>
+      <c r="F88" s="5" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="G88" s="6">
+        <f>IF(E88&gt;1,(1.732*D88*F88)/1000,(D88*F88)/1000)</f>
+        <v/>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>MOBILE</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>86</v>
-      </c>
-      <c r="B89" t="n">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>SOILED DISH TABLE</t>
+          <t>SPARE NUMBER</t>
         </is>
       </c>
       <c r="F89" s="5" t="n"/>
@@ -2534,98 +2553,96 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B90" t="n">
         <v>1</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>UNDERCOUNTER DISHWASHER</t>
-        </is>
-      </c>
-      <c r="D90" t="n">
-        <v>120</v>
-      </c>
-      <c r="E90" t="n">
-        <v>1</v>
-      </c>
-      <c r="F90" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="G90" s="6">
-        <f>IF(E90&gt;1,(1.732*D90*F90)/1000,(D90*F90)/1000)</f>
-        <v/>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>3/8"</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>6.5"</t>
-        </is>
-      </c>
+          <t>SOILED DISH TABLE</t>
+        </is>
+      </c>
+      <c r="F90" s="5" t="n"/>
+      <c r="G90" s="6" t="n"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B91" t="n">
         <v>1</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>HAND SINK</t>
-        </is>
-      </c>
-      <c r="F91" s="5" t="n"/>
-      <c r="G91" s="6" t="n"/>
+          <t>UNDERCOUNTER DISHWASHER</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>120</v>
+      </c>
+      <c r="E91" t="n">
+        <v>1</v>
+      </c>
+      <c r="F91" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="G91" s="6">
+        <f>IF(E91&gt;1,(1.732*D91*F91)/1000,(D91*F91)/1000)</f>
+        <v/>
+      </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>1/2"</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>1/2"</t>
-        </is>
-      </c>
-      <c r="J91" t="n">
-        <v>5</v>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>1-1/2"</t>
-        </is>
-      </c>
-      <c r="S91" t="inlineStr">
-        <is>
-          <t>WITH VENDOR PROVIDED SOAP &amp; TOWEL DISPENSER</t>
+          <t>3/8"</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>6.5"</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>89</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>88</v>
+      </c>
+      <c r="B92" t="n">
+        <v>1</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
+          <t>HAND SINK</t>
         </is>
       </c>
       <c r="F92" s="5" t="n"/>
       <c r="G92" s="6" t="n"/>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>1/2"</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>1/2"</t>
+        </is>
+      </c>
+      <c r="J92" t="n">
+        <v>5</v>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>1-1/2"</t>
+        </is>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>WITH VENDOR PROVIDED SOAP &amp; TOWEL DISPENSER</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -2642,44 +2659,44 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>91</v>
-      </c>
-      <c r="B94" t="n">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>TRASH RECEPTACLE</t>
+          <t>SPARE NUMBER</t>
         </is>
       </c>
       <c r="F94" s="5" t="n"/>
       <c r="G94" s="6" t="n"/>
-      <c r="S94" t="inlineStr">
-        <is>
-          <t>SLIM JIM</t>
-        </is>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>92</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>91</v>
+      </c>
+      <c r="B95" t="n">
+        <v>1</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>SPARE NUMBER</t>
+          <t>TRASH RECEPTACLE</t>
         </is>
       </c>
       <c r="F95" s="5" t="n"/>
       <c r="G95" s="6" t="n"/>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>SLIM JIM</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -2696,7 +2713,7 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -2712,10 +2729,8 @@
       <c r="G97" s="6" t="n"/>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>95-100</t>
-        </is>
+      <c r="A98" t="n">
+        <v>94</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -2731,36 +2746,55 @@
       <c r="G98" s="6" t="n"/>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr"/>
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>95-100</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>SPARE NUMBER</t>
+        </is>
+      </c>
+      <c r="F99" s="5" t="n"/>
+      <c r="G99" s="6" t="n"/>
     </row>
     <row r="100">
-      <c r="A100" s="8" t="inlineStr">
+      <c r="A100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="8" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G100" s="9">
-        <f>SUM(G7:G99)</f>
-        <v/>
-      </c>
-      <c r="J100" s="9">
-        <f>SUM(J7:J99)</f>
-        <v/>
-      </c>
-      <c r="M100" s="9">
-        <f>SUM(M7:M99)</f>
-        <v/>
-      </c>
-      <c r="N100" s="9">
-        <f>SUM(N7:N99)</f>
-        <v/>
-      </c>
-      <c r="O100" s="9">
-        <f>SUM(O7:O99)</f>
-        <v/>
-      </c>
-      <c r="P100" s="9">
-        <f>SUM(P7:P99)</f>
+      <c r="G101" s="9">
+        <f>SUM(G7:G100)</f>
+        <v/>
+      </c>
+      <c r="J101" s="9">
+        <f>SUM(J7:J100)</f>
+        <v/>
+      </c>
+      <c r="M101" s="9">
+        <f>SUM(M7:M100)</f>
+        <v/>
+      </c>
+      <c r="N101" s="9">
+        <f>SUM(N7:N100)</f>
+        <v/>
+      </c>
+      <c r="O101" s="9">
+        <f>SUM(O7:O100)</f>
+        <v/>
+      </c>
+      <c r="P101" s="9">
+        <f>SUM(P7:P100)</f>
         <v/>
       </c>
     </row>

</xml_diff>